<commit_message>
Author               : Prateek Kapoor File Added           : Master Sheet for Batch.xlsx Description          : Curated the entire sheet
</commit_message>
<xml_diff>
--- a/Requirements/Documents/Excel Sheets/Master Sheet for Batch.xlsx
+++ b/Requirements/Documents/Excel Sheets/Master Sheet for Batch.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\NSKFDC APP\trunk\Requirements\Documents\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{44062B6B-E928-419F-9CDB-3B91AA317EEC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5000F589-1361-43BB-B131-F5743A8C7820}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="670" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="670" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="DropDown Values" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1 (2)" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="DropDown Values" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1 (2)" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,6 +120,80 @@
     <author>prateek kapoor</author>
   </authors>
   <commentList>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{F4C7C1C1-D91D-416F-B34F-EB785532DA05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Centre details
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{DB399AC7-2F03-4CFB-B6D4-84FDD211C769}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+centre details
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{B2762D90-6BE2-4C81-8122-1622BE06A739}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Candidate Details</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A12" authorId="0" shapeId="0" xr:uid="{F2686EC6-7C54-46F0-8D5B-B6C09DA76D89}">
       <text>
         <r>
@@ -192,6 +267,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="X26" authorId="0" shapeId="0" xr:uid="{25E2D42B-43A2-403E-AD19-98D60F700B93}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+relation type in db</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB26" authorId="0" shapeId="0" xr:uid="{59D48215-187F-42BC-9BD8-7BBA635AF41A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+complete address with block number and colony</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AD26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
@@ -253,6 +376,115 @@
     <author>prateek kapoor</author>
   </authors>
   <commentList>
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{70AA4A7A-2685-47BC-AF5E-400670FE645B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+relation type in db</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{A67F0A82-1E59-429C-8162-B794619EAB18}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+complete address with block number and colony</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF3" authorId="0" shapeId="0" xr:uid="{8A06B804-0240-4BDE-98FD-971CECE78D93}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+yes or no
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{2EA8DA7B-9075-4632-82FD-CE83E9A61A77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>prateek kapoor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+It is pass or not appear
+Payout will be given to candidates who are pass
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>prateek kapoor</author>
+  </authors>
+  <commentList>
     <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
@@ -309,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="981">
   <si>
     <t>FirstNameCandidate</t>
   </si>
@@ -3247,6 +3479,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Batch ID</t>
+  </si>
+  <si>
+    <t>Batch Details</t>
   </si>
 </sst>
 </file>
@@ -3741,7 +3979,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3896,9 +4134,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3920,6 +4155,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3938,29 +4175,20 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3980,6 +4208,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3990,8 +4227,37 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4310,7 +4576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB61"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BD4" sqref="BD4"/>
     </sheetView>
   </sheetViews>
@@ -4362,182 +4628,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="77"/>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="77"/>
-      <c r="BB1" s="77"/>
+      <c r="A1" s="78"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
     </row>
     <row r="2" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="77"/>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="77"/>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="77"/>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="77"/>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="77"/>
-      <c r="AV2" s="77"/>
-      <c r="AW2" s="77"/>
-      <c r="AX2" s="77"/>
-      <c r="AY2" s="77"/>
-      <c r="AZ2" s="77"/>
-      <c r="BA2" s="77"/>
-      <c r="BB2" s="77"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="78"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="78"/>
+      <c r="AO2" s="78"/>
+      <c r="AP2" s="78"/>
+      <c r="AQ2" s="78"/>
+      <c r="AR2" s="78"/>
+      <c r="AS2" s="78"/>
+      <c r="AT2" s="78"/>
+      <c r="AU2" s="78"/>
+      <c r="AV2" s="78"/>
+      <c r="AW2" s="78"/>
+      <c r="AX2" s="78"/>
+      <c r="AY2" s="78"/>
+      <c r="AZ2" s="78"/>
+      <c r="BA2" s="78"/>
+      <c r="BB2" s="78"/>
     </row>
     <row r="3" spans="1:54" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="80" t="s">
         <v>906</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="79"/>
-      <c r="Z3" s="79"/>
-      <c r="AA3" s="79"/>
-      <c r="AB3" s="79"/>
-      <c r="AC3" s="80" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
+      <c r="AA3" s="80"/>
+      <c r="AB3" s="80"/>
+      <c r="AC3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="81" t="s">
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="81"/>
+      <c r="AF3" s="81"/>
+      <c r="AG3" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="AH3" s="81"/>
-      <c r="AI3" s="81"/>
-      <c r="AJ3" s="81"/>
-      <c r="AK3" s="81"/>
-      <c r="AL3" s="81"/>
-      <c r="AM3" s="81"/>
-      <c r="AN3" s="81"/>
-      <c r="AO3" s="81"/>
-      <c r="AP3" s="81"/>
-      <c r="AQ3" s="81"/>
-      <c r="AR3" s="81"/>
-      <c r="AS3" s="81"/>
-      <c r="AT3" s="81"/>
-      <c r="AU3" s="81"/>
-      <c r="AV3" s="81"/>
-      <c r="AW3" s="78" t="s">
+      <c r="AH3" s="82"/>
+      <c r="AI3" s="82"/>
+      <c r="AJ3" s="82"/>
+      <c r="AK3" s="82"/>
+      <c r="AL3" s="82"/>
+      <c r="AM3" s="82"/>
+      <c r="AN3" s="82"/>
+      <c r="AO3" s="82"/>
+      <c r="AP3" s="82"/>
+      <c r="AQ3" s="82"/>
+      <c r="AR3" s="82"/>
+      <c r="AS3" s="82"/>
+      <c r="AT3" s="82"/>
+      <c r="AU3" s="82"/>
+      <c r="AV3" s="82"/>
+      <c r="AW3" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="AX3" s="78"/>
-      <c r="AY3" s="78"/>
-      <c r="AZ3" s="76" t="s">
+      <c r="AX3" s="79"/>
+      <c r="AY3" s="79"/>
+      <c r="AZ3" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="BA3" s="76"/>
-      <c r="BB3" s="76"/>
+      <c r="BA3" s="77"/>
+      <c r="BB3" s="77"/>
     </row>
     <row r="4" spans="1:54" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -7407,8 +7673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView topLeftCell="R17" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="U17" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:AF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7448,17 +7714,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="83" t="s">
         <v>938</v>
       </c>
-      <c r="B1" s="89"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="68" t="s">
         <v>940</v>
       </c>
       <c r="B2" s="59" t="str">
@@ -7476,10 +7742,10 @@
       <c r="A3" s="41" t="s">
         <v>909</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>918</v>
       </c>
-      <c r="C3" s="93"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="62"/>
       <c r="E3" s="63"/>
       <c r="F3" s="63"/>
@@ -7488,10 +7754,10 @@
       <c r="A4" s="42" t="s">
         <v>910</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="92" t="s">
         <v>939</v>
       </c>
-      <c r="C4" s="95"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="62"/>
       <c r="E4" s="63"/>
       <c r="F4" s="63"/>
@@ -7500,10 +7766,10 @@
       <c r="A5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="92" t="s">
         <v>941</v>
       </c>
-      <c r="C5" s="95"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="64"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
@@ -7512,8 +7778,8 @@
       <c r="A6" s="42" t="s">
         <v>911</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="64"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -7522,8 +7788,8 @@
       <c r="A7" s="35" t="s">
         <v>912</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="91"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
@@ -7578,43 +7844,43 @@
       <c r="E12" s="65"/>
       <c r="F12" s="65"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>943</v>
       </c>
       <c r="B13" s="51"/>
       <c r="C13" s="52"/>
-      <c r="D13" s="68"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="63"/>
       <c r="F13" s="63"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>913</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="46"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="62"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>914</v>
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="46"/>
-      <c r="D15" s="68"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="65"/>
       <c r="F15" s="65"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>915</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="52"/>
-      <c r="D16" s="67"/>
+      <c r="D16" s="64"/>
       <c r="E16" s="63"/>
       <c r="F16" s="63"/>
     </row>
@@ -7624,9 +7890,9 @@
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="52"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
@@ -7636,9 +7902,9 @@
         <v>937</v>
       </c>
       <c r="C18" s="56"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
     </row>
     <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
@@ -7646,9 +7912,9 @@
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="52"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
@@ -7656,9 +7922,9 @@
       </c>
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B21" s="48"/>
@@ -7685,51 +7951,51 @@
       <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="82" t="s">
+      <c r="D24" s="85" t="s">
         <v>945</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
       <c r="K24" s="87"/>
-      <c r="L24" s="84" t="s">
+      <c r="L24" s="94" t="s">
         <v>948</v>
       </c>
-      <c r="M24" s="85"/>
-      <c r="N24" s="86"/>
-      <c r="O24" s="82" t="s">
+      <c r="M24" s="95"/>
+      <c r="N24" s="96"/>
+      <c r="O24" s="85" t="s">
         <v>949</v>
       </c>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
-      <c r="R24" s="83"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="86"/>
+      <c r="R24" s="86"/>
       <c r="S24" s="87"/>
-      <c r="T24" s="82" t="s">
+      <c r="T24" s="85" t="s">
         <v>949</v>
       </c>
-      <c r="U24" s="83"/>
-      <c r="V24" s="83"/>
-      <c r="W24" s="82" t="s">
+      <c r="U24" s="86"/>
+      <c r="V24" s="86"/>
+      <c r="W24" s="85" t="s">
         <v>949</v>
       </c>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
-      <c r="Z24" s="82" t="s">
+      <c r="X24" s="86"/>
+      <c r="Y24" s="86"/>
+      <c r="Z24" s="85" t="s">
         <v>949</v>
       </c>
-      <c r="AA24" s="83"/>
-      <c r="AB24" s="83"/>
-      <c r="AC24" s="82" t="s">
+      <c r="AA24" s="86"/>
+      <c r="AB24" s="86"/>
+      <c r="AC24" s="85" t="s">
         <v>949</v>
       </c>
-      <c r="AD24" s="83"/>
-      <c r="AE24" s="83"/>
-      <c r="AF24" s="101"/>
-      <c r="AG24" s="100"/>
-      <c r="AH24" s="100"/>
+      <c r="AD24" s="86"/>
+      <c r="AE24" s="86"/>
+      <c r="AF24" s="76"/>
+      <c r="AG24" s="75"/>
+      <c r="AH24" s="75"/>
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7739,90 +8005,90 @@
       <c r="E26" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F26" s="69" t="s">
         <v>946</v>
       </c>
-      <c r="G26" s="70" t="s">
+      <c r="G26" s="69" t="s">
         <v>947</v>
       </c>
-      <c r="H26" s="70" t="s">
+      <c r="H26" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="70" t="s">
+      <c r="I26" s="69" t="s">
         <v>921</v>
       </c>
-      <c r="J26" s="70" t="s">
+      <c r="J26" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="70" t="s">
+      <c r="K26" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="70" t="s">
+      <c r="L26" s="69" t="s">
         <v>922</v>
       </c>
-      <c r="M26" s="70" t="s">
+      <c r="M26" s="69" t="s">
         <v>923</v>
       </c>
-      <c r="N26" s="70" t="s">
+      <c r="N26" s="69" t="s">
         <v>924</v>
       </c>
-      <c r="O26" s="70" t="s">
+      <c r="O26" s="69" t="s">
         <v>950</v>
       </c>
-      <c r="P26" s="70" t="s">
+      <c r="P26" s="69" t="s">
         <v>853</v>
       </c>
-      <c r="Q26" s="70" t="s">
+      <c r="Q26" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="R26" s="70" t="s">
+      <c r="R26" s="69" t="s">
         <v>951</v>
       </c>
-      <c r="S26" s="70" t="s">
+      <c r="S26" s="69" t="s">
         <v>928</v>
       </c>
-      <c r="T26" s="70" t="s">
+      <c r="T26" s="69" t="s">
         <v>953</v>
       </c>
-      <c r="U26" s="70" t="s">
+      <c r="U26" s="69" t="s">
         <v>952</v>
       </c>
-      <c r="V26" s="70" t="s">
+      <c r="V26" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="W26" s="71" t="s">
+      <c r="W26" s="70" t="s">
         <v>954</v>
       </c>
-      <c r="X26" s="71" t="s">
+      <c r="X26" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="Y26" s="71" t="s">
+      <c r="Y26" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Z26" s="71" t="s">
+      <c r="Z26" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="AA26" s="71" t="s">
+      <c r="AA26" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="AB26" s="71" t="s">
+      <c r="AB26" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="AC26" s="71" t="s">
+      <c r="AC26" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="AD26" s="71" t="s">
+      <c r="AD26" s="70" t="s">
         <v>930</v>
       </c>
-      <c r="AE26" s="71" t="s">
+      <c r="AE26" s="70" t="s">
         <v>975</v>
       </c>
-      <c r="AF26" s="72" t="s">
+      <c r="AF26" s="71" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="60" x14ac:dyDescent="0.25">
-      <c r="D27" s="75">
+      <c r="D27" s="74">
         <v>1</v>
       </c>
       <c r="E27" s="51" t="s">
@@ -7840,7 +8106,7 @@
       <c r="I27" s="51" t="s">
         <v>884</v>
       </c>
-      <c r="J27" s="73">
+      <c r="J27" s="72">
         <v>32172</v>
       </c>
       <c r="K27" s="55" t="s">
@@ -7855,7 +8121,7 @@
       <c r="N27" s="51" t="s">
         <v>961</v>
       </c>
-      <c r="O27" s="74" t="s">
+      <c r="O27" s="73" t="s">
         <v>962</v>
       </c>
       <c r="P27" s="51" t="s">
@@ -7974,6 +8240,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="Z24:AB24"/>
+    <mergeCell ref="AC24:AE24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="O24:S24"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D24:K24"/>
     <mergeCell ref="B7:C7"/>
@@ -7981,12 +8253,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="Z24:AB24"/>
-    <mergeCell ref="AC24:AE24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="O24:S24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7995,6 +8261,360 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE5C98F-528E-4722-8922-B8ED1AD70BBF}">
+  <dimension ref="A1:AH6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="85" t="s">
+        <v>945</v>
+      </c>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="94" t="s">
+        <v>948</v>
+      </c>
+      <c r="O1" s="95"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="85" t="s">
+        <v>949</v>
+      </c>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="85" t="s">
+        <v>949</v>
+      </c>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="85" t="s">
+        <v>949</v>
+      </c>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="85" t="s">
+        <v>949</v>
+      </c>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="85" t="s">
+        <v>949</v>
+      </c>
+      <c r="AF1" s="86"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="76"/>
+    </row>
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:34" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="101" t="s">
+        <v>979</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>909</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>911</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>910</v>
+      </c>
+      <c r="F3" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="104" t="s">
+        <v>946</v>
+      </c>
+      <c r="I3" s="104" t="s">
+        <v>947</v>
+      </c>
+      <c r="J3" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="104" t="s">
+        <v>921</v>
+      </c>
+      <c r="L3" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="104" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="104" t="s">
+        <v>922</v>
+      </c>
+      <c r="O3" s="104" t="s">
+        <v>923</v>
+      </c>
+      <c r="P3" s="104" t="s">
+        <v>924</v>
+      </c>
+      <c r="Q3" s="104" t="s">
+        <v>950</v>
+      </c>
+      <c r="R3" s="104" t="s">
+        <v>853</v>
+      </c>
+      <c r="S3" s="104" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="104" t="s">
+        <v>951</v>
+      </c>
+      <c r="U3" s="104" t="s">
+        <v>928</v>
+      </c>
+      <c r="V3" s="104" t="s">
+        <v>953</v>
+      </c>
+      <c r="W3" s="104" t="s">
+        <v>952</v>
+      </c>
+      <c r="X3" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="105" t="s">
+        <v>954</v>
+      </c>
+      <c r="Z3" s="105" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="105" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE3" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF3" s="105" t="s">
+        <v>930</v>
+      </c>
+      <c r="AG3" s="105" t="s">
+        <v>975</v>
+      </c>
+      <c r="AH3" s="106" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="107"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="101">
+        <v>1</v>
+      </c>
+      <c r="G4" s="108" t="s">
+        <v>956</v>
+      </c>
+      <c r="H4" s="108" t="s">
+        <v>955</v>
+      </c>
+      <c r="I4" s="108" t="s">
+        <v>957</v>
+      </c>
+      <c r="J4" s="108" t="s">
+        <v>958</v>
+      </c>
+      <c r="K4" s="108" t="s">
+        <v>884</v>
+      </c>
+      <c r="L4" s="109">
+        <v>32172</v>
+      </c>
+      <c r="M4" s="110" t="s">
+        <v>959</v>
+      </c>
+      <c r="N4" s="108" t="s">
+        <v>960</v>
+      </c>
+      <c r="O4" s="108" t="s">
+        <v>957</v>
+      </c>
+      <c r="P4" s="108" t="s">
+        <v>961</v>
+      </c>
+      <c r="Q4" s="111" t="s">
+        <v>962</v>
+      </c>
+      <c r="R4" s="108" t="s">
+        <v>963</v>
+      </c>
+      <c r="S4" s="108" t="s">
+        <v>260</v>
+      </c>
+      <c r="T4" s="108" t="s">
+        <v>964</v>
+      </c>
+      <c r="U4" s="108" t="s">
+        <v>965</v>
+      </c>
+      <c r="V4" s="108" t="s">
+        <v>966</v>
+      </c>
+      <c r="W4" s="108" t="s">
+        <v>967</v>
+      </c>
+      <c r="X4" s="108" t="s">
+        <v>968</v>
+      </c>
+      <c r="Y4" s="108" t="s">
+        <v>873</v>
+      </c>
+      <c r="Z4" s="108" t="s">
+        <v>969</v>
+      </c>
+      <c r="AA4" s="110" t="s">
+        <v>970</v>
+      </c>
+      <c r="AB4" s="110" t="s">
+        <v>971</v>
+      </c>
+      <c r="AC4" s="110">
+        <v>123456789</v>
+      </c>
+      <c r="AD4" s="110" t="s">
+        <v>972</v>
+      </c>
+      <c r="AE4" s="110" t="s">
+        <v>973</v>
+      </c>
+      <c r="AF4" s="108" t="s">
+        <v>974</v>
+      </c>
+      <c r="AG4" s="110" t="s">
+        <v>976</v>
+      </c>
+      <c r="AH4" s="110" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="107"/>
+      <c r="Q5" s="107"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="107"/>
+      <c r="X5" s="107"/>
+      <c r="Y5" s="107"/>
+      <c r="Z5" s="107"/>
+      <c r="AA5" s="107"/>
+      <c r="AB5" s="107"/>
+      <c r="AC5" s="107"/>
+      <c r="AD5" s="107"/>
+      <c r="AE5" s="107"/>
+      <c r="AF5" s="107"/>
+      <c r="AG5" s="107"/>
+      <c r="AH5" s="107"/>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="107"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
+      <c r="Q6" s="107"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="107"/>
+      <c r="T6" s="107"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="107"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="107"/>
+      <c r="Z6" s="107"/>
+      <c r="AA6" s="107"/>
+      <c r="AB6" s="107"/>
+      <c r="AC6" s="107"/>
+      <c r="AD6" s="107"/>
+      <c r="AE6" s="107"/>
+      <c r="AF6" s="107"/>
+      <c r="AG6" s="107"/>
+      <c r="AH6" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I860"/>
   <sheetViews>
@@ -8043,7 +8663,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -8072,7 +8692,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="100"/>
       <c r="B3" s="2" t="s">
         <v>89</v>
       </c>
@@ -8221,7 +8841,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="97" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -8235,7 +8855,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="2" t="s">
         <v>98</v>
       </c>
@@ -8244,7 +8864,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="99" t="s">
         <v>66</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -8255,7 +8875,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="97"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="2" t="s">
         <v>100</v>
       </c>
@@ -12587,11 +13207,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>